<commit_message>
Progress on DS 775 Wk 10
</commit_message>
<xml_diff>
--- a/wk10/HW_10_Isaacson.xlsx
+++ b/wk10/HW_10_Isaacson.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="20.1-1" sheetId="1" r:id="rId1"/>
     <sheet name="20.1-2" sheetId="2" r:id="rId2"/>
     <sheet name="20.1-3" sheetId="3" r:id="rId3"/>
     <sheet name="20.4-11" sheetId="4" r:id="rId4"/>
+    <sheet name="20.6-2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="RandomNumber">'20.1-1'!$D$13:$D$62</definedName>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>20.1-1</t>
   </si>
@@ -183,6 +184,57 @@
   </si>
   <si>
     <t>20.4-11</t>
+  </si>
+  <si>
+    <t>20.6-2</t>
+  </si>
+  <si>
+    <t>cost to purchase</t>
+  </si>
+  <si>
+    <t>construction</t>
+  </si>
+  <si>
+    <t>triangle</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>distrbution</t>
+  </si>
+  <si>
+    <t>annual profit</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>2,3,4,5</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>4000-8000</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End of Year </t>
+  </si>
+  <si>
+    <t>Net</t>
   </si>
 </sst>
 </file>
@@ -227,7 +279,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +343,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,6 +357,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -640,20 +699,20 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.06640625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
@@ -664,26 +723,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C3">
-        <v>0.69044584892060346</v>
+        <v>0.3039</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>IF(C3&lt;0.5,"Heads","Tails")</f>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>IF(C3&lt;0.6,"Strike","Ball")</f>
-        <v>Ball</v>
+        <v>Strike</v>
       </c>
       <c r="F3" s="1" t="str">
         <f>IF(C3&lt;0.4,"Green",IF(AND(C3&gt;=0.4, C3 &lt; 0.5), "Yellow", "Red"))</f>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>Green</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4">
-        <v>0.50349254143381983</v>
+        <v>0.79139999999999999</v>
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" ref="D4:D8" si="0">IF(C4&lt;0.5,"Heads","Tails")</f>
@@ -691,16 +750,16 @@
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" ref="E4:E8" si="1">IF(C4&lt;0.6,"Strike","Ball")</f>
-        <v>Strike</v>
+        <v>Ball</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" ref="F4:F8" si="2">IF(C4&lt;0.4,"Green",IF(AND(C4&gt;=0.4, C4 &lt; 0.5), "Yellow", "Red"))</f>
         <v>Red</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5">
-        <v>0.97038150097019393</v>
+        <v>0.85429999999999995</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -715,9 +774,9 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6">
-        <v>0.95305408609689535</v>
+        <v>0.69020000000000004</v>
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -732,9 +791,9 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7">
-        <v>0.44857096190948043</v>
+        <v>0.3004</v>
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -746,35 +805,35 @@
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Yellow</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>Green</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8">
-        <v>0.72790420070021522</v>
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Tails</v>
+        <v>Heads</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Ball</v>
+        <v>Strike</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+        <v>Green</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
@@ -787,20 +846,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.46484375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -808,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -831,7 +890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -855,7 +914,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -879,7 +938,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -903,7 +962,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -927,7 +986,7 @@
         <v>Rain</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -951,7 +1010,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -975,7 +1034,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
@@ -999,7 +1058,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
@@ -1023,7 +1082,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
@@ -1047,7 +1106,7 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -1071,12 +1130,12 @@
         <v>Clear</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
@@ -1099,13 +1158,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <f ca="1">RAND()</f>
-        <v>0.96375151846630447</v>
+        <v>0.3004</v>
       </c>
       <c r="D17" s="4" t="str">
         <f>C15</f>
@@ -1120,233 +1178,224 @@
         <v>0.8</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" ref="G17:G26" ca="1" si="4">IF(C17&lt;E17,"Rain", "Clear")</f>
-        <v>Clear</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+        <f>IF(C17&lt;E17,"Rain", "Clear")</f>
+        <v>Clear</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:C26" ca="1" si="5">RAND()</f>
-        <v>0.91127895584630414</v>
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="D18" s="4" t="str">
-        <f t="shared" ref="D18:D26" ca="1" si="6">G17</f>
+        <f t="shared" ref="D18:D26" si="4">G17</f>
         <v>Clear</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:E26" ca="1" si="7">IF($D18="Rain",0.6, 0.2)</f>
+        <f t="shared" ref="E18:E26" si="5">IF($D18="Rain",0.6, 0.2)</f>
         <v>0.2</v>
       </c>
       <c r="F18">
-        <f t="shared" ref="F18:F26" ca="1" si="8">IF($D18="Clear",0.8,0.4)</f>
+        <f t="shared" ref="F18:F26" si="6">IF($D18="Clear",0.8,0.4)</f>
         <v>0.8</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Clear</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" ref="G18:G26" si="7">IF(C18&lt;E18,"Rain", "Clear")</f>
+        <v>Rain</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>3</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.37994303786397521</v>
+        <v>0.38829999999999998</v>
       </c>
       <c r="D19" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Clear</v>
+        <f t="shared" si="4"/>
+        <v>Rain</v>
       </c>
       <c r="E19">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.2</v>
+        <f t="shared" si="5"/>
+        <v>0.6</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.8</v>
+        <f t="shared" si="6"/>
+        <v>0.4</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Clear</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" si="7"/>
+        <v>Rain</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.61693159962048627</v>
+        <v>0.60519999999999996</v>
       </c>
       <c r="D20" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Clear</v>
+        <f t="shared" si="4"/>
+        <v>Rain</v>
       </c>
       <c r="E20">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.2</v>
+        <f t="shared" si="5"/>
+        <v>0.6</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.8</v>
+        <f t="shared" si="6"/>
+        <v>0.4</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Clear</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" si="7"/>
+        <v>Clear</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="5"/>
-        <v>2.5289196886122745E-2</v>
+        <v>0.22309999999999999</v>
       </c>
       <c r="D21" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" si="4"/>
         <v>Clear</v>
       </c>
       <c r="E21">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Rain</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" si="7"/>
+        <v>Clear</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>6</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.29174646172420304</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="D22" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Rain</v>
+        <f t="shared" si="4"/>
+        <v>Clear</v>
       </c>
       <c r="E22">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.6</v>
+        <f t="shared" si="5"/>
+        <v>0.2</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.4</v>
+        <f t="shared" si="6"/>
+        <v>0.8</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Rain</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" si="7"/>
+        <v>Clear</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>7</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.62594110984028162</v>
+        <v>0.37290000000000001</v>
       </c>
       <c r="D23" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Rain</v>
+        <f t="shared" si="4"/>
+        <v>Clear</v>
       </c>
       <c r="E23">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.6</v>
+        <f t="shared" si="5"/>
+        <v>0.2</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.4</v>
+        <f t="shared" si="6"/>
+        <v>0.8</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Clear</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" si="7"/>
+        <v>Clear</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>8</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.38937781175762531</v>
+        <v>0.79830000000000001</v>
       </c>
       <c r="D24" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" si="4"/>
         <v>Clear</v>
       </c>
       <c r="E24">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Clear</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" si="7"/>
+        <v>Clear</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>9</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.81183727540244233</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="D25" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" si="4"/>
         <v>Clear</v>
       </c>
       <c r="E25">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Clear</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
+        <f t="shared" si="7"/>
+        <v>Clear</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>10</v>
       </c>
       <c r="C26">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.41295639188092814</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="D26" s="4" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" si="4"/>
         <v>Clear</v>
       </c>
       <c r="E26">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="F26">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Clear</v>
+        <f t="shared" si="7"/>
+        <v>Rain</v>
       </c>
     </row>
   </sheetData>
@@ -1372,21 +1421,21 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="6.265625" customWidth="1"/>
-    <col min="9" max="9" width="13.19921875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
         <v>15</v>
       </c>
@@ -1406,7 +1455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -1430,7 +1479,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1455,7 +1504,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>D5</f>
         <v>0.16</v>
@@ -1477,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1506,7 +1555,7 @@
         <v>3.6800000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1514,11 +1563,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>15</v>
       </c>
@@ -1532,13 +1581,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C12">
         <f ca="1">RAND()</f>
-        <v>0.70868605117360828</v>
+        <v>0.99527974302949673</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1558,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>3</v>
       </c>
@@ -1577,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>4</v>
       </c>
@@ -1589,14 +1638,14 @@
       </c>
       <c r="G14" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>5</v>
       </c>
@@ -1615,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>6</v>
       </c>
@@ -1627,21 +1676,21 @@
       </c>
       <c r="G16" t="b">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="e">
         <f ca="1">SUM(H12:H16) + _xll.PsiOutput()</f>
-        <v>4</v>
+        <v>#NAME?</v>
       </c>
       <c r="I17" t="e">
         <f ca="1">_xll.PsiMean(H17)</f>
-        <v>#N/A</v>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -1653,25 +1702,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.265625" customWidth="1"/>
-    <col min="4" max="4" width="10.796875" customWidth="1"/>
-    <col min="5" max="8" width="6.265625" customWidth="1"/>
-    <col min="9" max="9" width="13.19921875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>15</v>
       </c>
@@ -1685,11 +1734,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4">
         <f ca="1">RAND()</f>
-        <v>0.65432685346749375</v>
+        <v>0.42112564724262325</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -1709,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>9</v>
       </c>
@@ -1728,7 +1777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>11</v>
       </c>
@@ -1747,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>13</v>
       </c>
@@ -1761,6 +1810,193 @@
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>700</v>
+      </c>
+      <c r="D5">
+        <v>700</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>-1000</v>
+      </c>
+      <c r="L10">
+        <f>J10+K10</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9">
+        <v>-2000</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L15" si="0">J11+K11</f>
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12" s="9">
+        <v>700</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13" s="9">
+        <v>700</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14" s="9">
+        <v>700</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15" s="9">
+        <v>700</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f>SUM(L10:L15)</f>
+        <v>-200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>